<commit_message>
score tab + multiple fixes + ws notification when other people are playing
</commit_message>
<xml_diff>
--- a/datamodel/resources/data/characters.xlsx
+++ b/datamodel/resources/data/characters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pde-rent\Projects\monisnap_assessment\datamodel\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34943949-C507-49D3-9C9C-E9F05E5461C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB00E2A-5BF3-4807-A572-4B987ABBF416}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1581,10 +1581,10 @@
   <dimension ref="A1:N87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G60" sqref="G60"/>
+      <selection pane="bottomRight" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3083,7 +3083,7 @@
         <v>13</v>
       </c>
       <c r="I32" t="s">
-        <v>224</v>
+        <v>92</v>
       </c>
       <c r="J32" t="s">
         <v>15</v>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="N32" t="str">
         <f>"('"&amp;Table2[[#This Row],[name]]&amp;"',"&amp;Table2[[#This Row],[height]]&amp;","&amp;Table2[[#This Row],[mass]]&amp;",'"&amp;UPPER(Table2[[#This Row],[hair_color]])&amp;"','"&amp;UPPER(Table2[[#This Row],[skin_color]])&amp;"','"&amp;UPPER(Table2[[#This Row],[eye_color]])&amp;"',"&amp;Table2[[#This Row],[birth_year (BY)]]&amp;",'"&amp;UPPER(Table2[[#This Row],[gender]])&amp;"', public.planet_name_to_id('"&amp;Table2[[#This Row],[homeworld]]&amp;"'), public.species_name_to_id('"&amp;Table2[[#This Row],[species]]&amp;"'),'"&amp;UPPER(Table2[[#This Row],[main affiliation]])&amp;"'),"</f>
-        <v>('Qui-Gon Jinn',193,89,'BROWN','FAIR','BLUE',-92,'MALE', public.planet_name_to_id('Unknown'), public.species_name_to_id('Human'),'JEDI_ORDER'),</v>
+        <v>('Qui-Gon Jinn',193,89,'BROWN','FAIR','BLUE',-92,'MALE', public.planet_name_to_id('Coruscant'), public.species_name_to_id('Human'),'JEDI_ORDER'),</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>